<commit_message>
added to parts excel
</commit_message>
<xml_diff>
--- a/boards/on-robot/kicker-v4.1/kicker_parts.xlsx
+++ b/boards/on-robot/kicker-v4.1/kicker_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellamcchesney/Desktop/Coding/roboCup/robocup-pcb/boards/on-robot/kicker-v4.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B4A95F-7935-B349-935C-F48944B40A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B132CA7-915E-214E-9C0A-F4E6F5CD8CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="27600" windowHeight="16940" xr2:uid="{95D6933F-B380-1345-BC2E-5F4C9E06552B}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="295">
   <si>
     <t>Qty</t>
   </si>
@@ -859,13 +859,97 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H2ATTD2943F/10234483</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/PWR263S-35-1501F?qs=ZVKuL1Ob8AvWpO608Z7NmQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/MCT0603PD1003DP500/7245012</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RNCP0603FTD10K0/2240139</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B106KBJNNWE/3889046</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B106KLJNNNE/3889047</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/MCT06030C1600FP500/7347856</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF1206FT160R/1759117</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRT188R6YA225KE13D/5416757</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805JT22R0/1757897</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/C0805C221K1RAC7800/2212222</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CC0603MRX5R6BB226/5195226</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/C2012X5R1V226M125AC/3951664</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0805FR-0725K5L/727768</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603FR-07270KL/727104</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0353630360/755311?s=N4IgTCBcDaIO4FsCMAOAnAZjAWgHYBMQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/MCT06030D3001BP500/462683</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/RCS060330K1FKEA/5868643</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ331/1762730</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/742C163331JP/742C163331JPCT-ND/1124503?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H2ATTD4123F/10234127</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT43K2/1761153</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RN73H1JTTD5053B50/10677157</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPF51R0/1983446</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/TLRH3APTTE7L00F/9856512</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/VLMB1300-GS08/3025494</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C191KGKT/386835</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C191KRKT/386837</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C194KSKT/2356224</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -880,6 +964,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -903,9 +999,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1227,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E204FEF4-CD2B-6B4C-8340-FC6B854F92E5}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,1735 +1343,2091 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="H5" t="s">
-        <v>222</v>
-      </c>
+      <c r="H5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="H6" t="s">
-        <v>222</v>
-      </c>
+      <c r="H6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="H7" t="s">
-        <v>222</v>
-      </c>
+      <c r="H7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H8" t="s">
-        <v>222</v>
-      </c>
+      <c r="H8" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H10" t="s">
-        <v>222</v>
-      </c>
+      <c r="H10" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="H16" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="H17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="H17" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="H18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="H18" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="H19" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="H20" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G21" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>160</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="G22" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>2</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>160</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="G23" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H24" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="H24" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="H25" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H26" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="H26" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="H27" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="H27" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G28" t="s">
+      <c r="F28" s="3"/>
+      <c r="G28" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="H28" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30">
+      <c r="G29" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
         <v>22</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="G30" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="G31" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="G32" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="G33" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>2</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="G34" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="G35" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H36" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="H36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F37" s="3"/>
+      <c r="G37" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="G38" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="G39" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>3</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>330</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41">
+      <c r="G40" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2">
         <v>330</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="G41" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H42" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="H42" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="G43" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45">
+      <c r="G44" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2">
         <v>500</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G45" t="s">
+      <c r="F45" s="3"/>
+      <c r="G45" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="H45" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47">
+      <c r="G46" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2">
         <v>51</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="G47" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="G48" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G49" t="s">
-        <v>246</v>
-      </c>
-      <c r="H49" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="G49" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G50" t="s">
+      <c r="F50" s="3"/>
+      <c r="G50" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="H50" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G51" t="s">
+      <c r="F51" s="3"/>
+      <c r="G51" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="H51" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="H51" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>1</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G52" t="s">
+      <c r="F52" s="3"/>
+      <c r="G52" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H52" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="H52" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G53" t="s">
+      <c r="F53" s="3"/>
+      <c r="G53" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="H53" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="H53" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G54" t="s">
+      <c r="F54" s="3"/>
+      <c r="G54" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="H54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
         <v>3</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="H55" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
         <v>2</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="F56" s="3"/>
+      <c r="G56" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>4</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G57" t="s">
+      <c r="F57" s="3"/>
+      <c r="G57" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H57" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="H57" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>1</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G58" t="s">
+      <c r="F58" s="3"/>
+      <c r="G58" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H58" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="H58" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>1</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G59" t="s">
+      <c r="F59" s="3"/>
+      <c r="G59" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H59" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="H59" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>1</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G60" t="s">
+      <c r="F60" s="3"/>
+      <c r="G60" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H60" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="H60" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="H61" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="H61" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
         <v>4</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="H62" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>1</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="H62" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>1</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H63" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="H63" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
         <v>4</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="F64" s="3"/>
+      <c r="G64" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
         <v>3</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G65" t="s">
+      <c r="F65" s="3"/>
+      <c r="G65" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="H65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>1</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="H65" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>1</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G66" t="s">
+      <c r="F66" s="3"/>
+      <c r="G66" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H66" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="H66" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>1</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G67" t="s">
+      <c r="F67" s="3"/>
+      <c r="G67" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H67" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>1</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="H67" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>1</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G68" t="s">
+      <c r="F68" s="3"/>
+      <c r="G68" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H68" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="H68" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
         <v>2</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G69" t="s">
+      <c r="F69" s="3"/>
+      <c r="G69" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="H69" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>1</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="H69" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>1</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G70" t="s">
+      <c r="F70" s="3"/>
+      <c r="G70" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>1</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G71" t="s">
+      <c r="F71" s="3"/>
+      <c r="G71" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H71" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="H71" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>1</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H72" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>1</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="H72" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>1</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H73" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="H73" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
         <v>4</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="F74" s="3"/>
+      <c r="G74" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
         <v>2</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G75" t="s">
+      <c r="F75" s="3"/>
+      <c r="G75" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H75" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="H75" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
         <v>3</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G76" t="s">
+      <c r="F76" s="3"/>
+      <c r="G76" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="H76" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="H76" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
         <v>4</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="2" t="s">
         <v>217</v>
       </c>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I77" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1" xr:uid="{ACCD43D9-1CCB-EA4F-8D24-784BF732E871}"/>
-    <hyperlink ref="G8" r:id="rId2" xr:uid="{33A09938-91CB-E345-A08A-736111264533}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{A57E7084-0BEB-F043-BBFD-B1F04667E85D}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{E2099EF7-E7D6-4A4A-B473-CE374F032CEE}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00D0F068-A6A5-2340-B7DB-E940F8665936}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{4E9DF2EC-492D-2444-A2BE-DCCCE39AA6E4}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{8010CAEC-2B98-D245-B3C7-6A7BE8C21813}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{EECCE212-7DC9-0A41-A790-046C5460A10D}"/>
+    <hyperlink ref="G11" r:id="rId7" xr:uid="{240E2953-EAB6-2C42-A6EF-D48ED90B613C}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{EA664E96-192D-DD46-B30A-C9AF654B5804}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{83B7EDB6-D5AF-B141-8254-344D8F977AF6}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{7FAA0354-419F-8A41-9806-84DECE1A8C43}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{C9636BC4-F5A9-FD4D-986B-AD76B27DF6D9}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{F6627BD6-33F4-844D-B1E4-F0C1F8D89360}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{7FF8F752-58BE-A943-BA1B-D81534E5A16F}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{66E5F278-DEDF-0D41-904A-4072C0095D0E}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{EF5FDD39-67FA-7E41-B85A-3DABE70524B7}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{3E561D7B-11FD-B043-82BB-5B617C37C751}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{0EA63309-B8F6-F543-80FC-C5F36FF354B1}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{4F8FA04F-E511-7242-B551-6907F3AF0569}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{1992E144-314B-564B-A404-A614072DA306}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{EE808593-40FC-0F45-84F8-440123715303}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{DA0A3083-00CD-5649-A5F6-37F11768124F}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{F6F16678-DAB3-FB49-B6B2-5E8D77B593CF}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{097B4434-88BC-7D41-9ADF-5C83022C3773}"/>
+    <hyperlink ref="G29" r:id="rId24" xr:uid="{078F8545-3252-3F49-BAA9-8FE291577A53}"/>
+    <hyperlink ref="G30" r:id="rId25" xr:uid="{1A8B84CD-73C0-1649-869C-3BF28325821B}"/>
+    <hyperlink ref="G31" r:id="rId26" xr:uid="{2977A9C9-8C57-1C43-A382-DBE50A77798C}"/>
+    <hyperlink ref="G32" r:id="rId27" xr:uid="{0C63E04D-5C2D-B24F-87BB-152F8A32D4FD}"/>
+    <hyperlink ref="G33" r:id="rId28" xr:uid="{00EAB4DD-03C9-A04C-B54F-2EAE5A6FF31E}"/>
+    <hyperlink ref="G34" r:id="rId29" xr:uid="{9934026E-0231-9C4C-8480-A4FFF0A65577}"/>
+    <hyperlink ref="G35" r:id="rId30" xr:uid="{713A5995-F670-4B45-ACB2-6CDC437ACC25}"/>
+    <hyperlink ref="G36" r:id="rId31" xr:uid="{309ACFA9-0722-0E4A-A276-CACE2C28B6BE}"/>
+    <hyperlink ref="G37" r:id="rId32" xr:uid="{25E21646-CBB4-124B-9B13-E07E8EB7195C}"/>
+    <hyperlink ref="G38" r:id="rId33" xr:uid="{96F79345-D772-AA4A-84E9-343106749024}"/>
+    <hyperlink ref="G39" r:id="rId34" xr:uid="{95E39576-D42E-F14A-9A28-CAF0D5B0594C}"/>
+    <hyperlink ref="G40" r:id="rId35" xr:uid="{DA0CCC3E-D355-BC4E-B0FB-6B1675176618}"/>
+    <hyperlink ref="G41" r:id="rId36" xr:uid="{949E2DDA-A3BA-D54C-A348-317A12F61A50}"/>
+    <hyperlink ref="G42" r:id="rId37" xr:uid="{A788F769-452F-B941-9AC4-4B4C346C3961}"/>
+    <hyperlink ref="G43" r:id="rId38" xr:uid="{BE06AD23-322D-6541-AE0C-AB38DEDFD7A1}"/>
+    <hyperlink ref="G44" r:id="rId39" xr:uid="{918ACBC9-E4AA-EE42-A648-84C6D64C5E27}"/>
+    <hyperlink ref="G45" r:id="rId40" xr:uid="{0F122322-EABB-FD4C-8CEC-3DE00A99F37B}"/>
+    <hyperlink ref="G46" r:id="rId41" xr:uid="{0A50892C-BE7A-C840-AFE5-E20006F3EAEF}"/>
+    <hyperlink ref="G47" r:id="rId42" xr:uid="{70A2C96B-DF5A-704C-A383-B2CFAF82DAC9}"/>
+    <hyperlink ref="G48" r:id="rId43" xr:uid="{9894E211-0996-D442-8F3F-F5022976C233}"/>
+    <hyperlink ref="G49" r:id="rId44" xr:uid="{921A1517-97B9-FB40-9922-44A96B963367}"/>
+    <hyperlink ref="G50" r:id="rId45" xr:uid="{E7C77679-EDC0-2545-B738-14526AA84CEE}"/>
+    <hyperlink ref="G51" r:id="rId46" xr:uid="{D528F957-4117-E946-A110-22FDB8287DFD}"/>
+    <hyperlink ref="G52" r:id="rId47" xr:uid="{2E63DCFF-4CBC-2148-9698-F1A3B0002612}"/>
+    <hyperlink ref="G53" r:id="rId48" xr:uid="{2A54AC92-7AEE-7F4B-AC23-5FF156D8860E}"/>
+    <hyperlink ref="G54" r:id="rId49" xr:uid="{64BAFEFA-E294-A844-97DF-9117E9F49AB7}"/>
+    <hyperlink ref="G55" r:id="rId50" xr:uid="{37836DA5-20F4-044B-8C01-BB2A5B7F0401}"/>
+    <hyperlink ref="G56" r:id="rId51" xr:uid="{ADC3F626-FE65-1946-9DC1-810419F71E8D}"/>
+    <hyperlink ref="G57" r:id="rId52" xr:uid="{352DD1C5-20DC-8D42-9086-85D5CF160647}"/>
+    <hyperlink ref="G58" r:id="rId53" xr:uid="{FA4236A6-0E00-B945-8D61-1512EE35202C}"/>
+    <hyperlink ref="G59" r:id="rId54" xr:uid="{F547A9F9-341D-6747-BA55-317C5670D494}"/>
+    <hyperlink ref="G60" r:id="rId55" xr:uid="{3113B3CB-8C61-3540-BD13-AD9B93F27CEF}"/>
+    <hyperlink ref="G61" r:id="rId56" xr:uid="{8E798DD9-6868-F041-988F-8C95FF2ADC0E}"/>
+    <hyperlink ref="G62" r:id="rId57" xr:uid="{4AB3C377-86BA-9E4E-9D04-50BB87EFFEDD}"/>
+    <hyperlink ref="G63" r:id="rId58" xr:uid="{E03F930A-AAF3-8241-BEF0-83127A81762E}"/>
+    <hyperlink ref="G64" r:id="rId59" xr:uid="{F340DFF3-544C-CA4E-82B6-B8F44F919844}"/>
+    <hyperlink ref="G65" r:id="rId60" xr:uid="{503CCDC6-2C38-9043-ABC0-5147737C12A4}"/>
+    <hyperlink ref="G66" r:id="rId61" xr:uid="{B7659D6D-B86A-514F-839B-2021984281BB}"/>
+    <hyperlink ref="G67" r:id="rId62" xr:uid="{5C7933AE-04A4-A143-BFAF-F80A76808BD7}"/>
+    <hyperlink ref="G68" r:id="rId63" xr:uid="{A2F0F1E5-5C3A-7246-A1ED-F1DAD531F686}"/>
+    <hyperlink ref="G69" r:id="rId64" xr:uid="{F138897B-690C-3344-9CFF-A5B856994207}"/>
+    <hyperlink ref="G70" r:id="rId65" location="PBF&amp;sn=Analog+Devices+Inc.&amp;utm_source=octopart&amp;utm_medium=aggregator&amp;utm_campaign=584-LT3751IFE%23PBF&amp;utm_content=Analog+Devices+Inc.&amp;exact=true" display="https://www.mouser.com/c/?q=584-LT3751IFE - PBF&amp;sn=Analog+Devices+Inc.&amp;utm_source=octopart&amp;utm_medium=aggregator&amp;utm_campaign=584-LT3751IFE%23PBF&amp;utm_content=Analog+Devices+Inc.&amp;exact=true" xr:uid="{94D93F8A-E8BA-9E45-B887-EF9B43285F41}"/>
+    <hyperlink ref="G71" r:id="rId66" xr:uid="{2F2B697F-9E38-9C4F-A02F-081CD8A56F1E}"/>
+    <hyperlink ref="G72" r:id="rId67" xr:uid="{B4201B9A-C200-9B46-9237-E6F4BE83313C}"/>
+    <hyperlink ref="G73" r:id="rId68" xr:uid="{8B1C07E4-9C3A-CC47-95BD-F97EC13089C6}"/>
+    <hyperlink ref="G74" r:id="rId69" xr:uid="{72BCB922-ABAA-A94C-AF13-9BE15AB61CED}"/>
+    <hyperlink ref="G75" r:id="rId70" xr:uid="{3071C9BA-CBBE-FA4F-97F3-E7FE3AC3AE57}"/>
+    <hyperlink ref="G76" r:id="rId71" xr:uid="{AE90E888-74CB-5147-8F95-04738E0C4C75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>